<commit_message>
Actualización Reto 4 y 5
</commit_message>
<xml_diff>
--- a/Reto 4/Maquetación solucion reto 4.xlsx
+++ b/Reto 4/Maquetación solucion reto 4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ProjectSupport\Documents\GitHub\Python\Reto 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E6B04C-0A1A-4AFB-BCD7-E16BFA1C8794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5654577E-ADFD-4A3B-9F89-5E67A38F653C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BCA33D8B-BFC3-4744-97DE-E77E8D039D78}"/>
+    <workbookView xWindow="2784" yWindow="5988" windowWidth="17280" windowHeight="7680" xr2:uid="{BCA33D8B-BFC3-4744-97DE-E77E8D039D78}"/>
   </bookViews>
   <sheets>
     <sheet name="Entrada" sheetId="3" r:id="rId1"/>
@@ -459,6 +459,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -484,9 +487,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -805,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1569121-F8DD-4253-B3F7-01AECAFAE877}">
   <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="G16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -828,17 +828,17 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:9" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="39"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="30"/>
     </row>
     <row r="3" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
@@ -994,16 +994,16 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:9" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="35"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="36"/>
     </row>
     <row r="11" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="20" t="s">
@@ -1150,21 +1150,21 @@
       <c r="A19" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="35"/>
-      <c r="K19" s="36" t="s">
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="36"/>
+      <c r="K19" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="L19" s="37"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="39"/>
       <c r="O19" s="25"/>
       <c r="P19" s="13" t="s">
         <v>18</v>
@@ -1360,16 +1360,16 @@
       <c r="P24" s="21"/>
     </row>
     <row r="25" spans="1:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K25" s="30" t="s">
+      <c r="K25" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="L25" s="31"/>
-      <c r="M25" s="31"/>
-      <c r="N25" s="32"/>
-      <c r="P25" s="30" t="s">
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="33"/>
+      <c r="P25" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="Q25" s="32"/>
+      <c r="Q25" s="33"/>
     </row>
     <row r="26" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="K26" s="12" t="s">

</xml_diff>